<commit_message>
Added scrolling, moved Test Status and Assignee, changed topnav, added help, corrected status buttons styling
</commit_message>
<xml_diff>
--- a/excel_test_cases.xlsx
+++ b/excel_test_cases.xlsx
@@ -80,7 +80,15 @@
     <t xml:space="preserve">Check filters</t>
   </si>
   <si>
-    <t xml:space="preserve">filters ok</t>
+    <t xml:space="preserve">filters ok
+ - name filter is okay
+ - date filter has datepicker field
+ - some othe
+Lorem ipsum odor amet, consectetuer adipiscing elit. Erat pulvinar aenean enim aptent libero a metus rhoncus? Leo posuere senectus; quis aptent sed egestas efficitur lectus. Felis libero fermentum erat iaculis consequat. Interdum placerat efficitur dignissim rhoncus a vivamus suscipit. Sit nostra ex fusce efficitur turpis. Nibh erat augue ligula aliquet ullamcorper tristique blandit urna praesent. Velit facilisi nostra quis fames nulla.
+Sapien eros feugiat lacinia hendrerit etiam duis nam netus suspendisse. Fames scelerisque cursus consequat ante neque mi mus etiam. Ridiculus arcu dictumst nascetur, porttitor cursus dictum rhoncus ultricies elementum. Dis dignissim odio quis ac ornare vivamus. Ullamcorper dui condimentum sodales nascetur ante velit. Cras montes id fermentum erat condimentum feugiat. Faucibus etiam nostra efficitur class tortor congue consectetur. Varius enim luctus suspendisse venenatis scelerisque suscipit aliquam inceptos suscipit.
+Rutrum risus vitae mollis interdum varius euismod hendrerit elementum. At dignissim vestibulum venenatis elementum id augue. Parturient netus lorem libero potenti efficitur. Pellentesque quisque torquent ac vehicula ante dictumst quam vehicula. Hac scelerisque nullam bibendum felis eu. Nascetur blandit integer ipsum et a nunc at magna curae. Commodo egestas praesent dictum vitae sed; fringilla eu nam.
+Bibendum adipiscing est ultrices aliquam mattis maximus feugiat convallis. Porta nullam lectus in hac rhoncus risus efficitur purus. Interdum conubia ad laoreet iaculis fames viverra. Dis maecenas in proin gravida eu ullamcorper eleifend rutrum. Congue in euismod dis fermentum vitae suscipit ornare. Inceptos senectus pharetra ad feugiat class suscipit.
+Quis quis mattis aptent bibendum nunc natoque, eros id. Erat nibh nullam nunc amet conubia morbi faucibus. Condimentum ligula placerat ut mattis feugiat. Etiam ex rutrum turpis pulvinar penatibus. Pharetra amet sagittis dapibus vestibulum amet; fames posuere habitant. Inceptos consequat sagittis facilisi per justo iaculis tristique. Vehicula nam sit placerat molestie parturient amet diam et. Netus diam hendrerit natoque; dolor ut interdum fringilla. Aptent commodo dapibus lectus taciti placerat, elementum augue in lacus.!</t>
   </si>
   <si>
     <t xml:space="preserve">check export</t>
@@ -227,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,8 +244,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -388,8 +400,8 @@
   </sheetPr>
   <dimension ref="A3:L16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -461,7 +473,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="2554.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -483,7 +495,7 @@
       <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>